<commit_message>
Added another big graph for the result section of our essay and presentation
</commit_message>
<xml_diff>
--- a/Results/Resulaten Tabel excel.xlsx
+++ b/Results/Resulaten Tabel excel.xlsx
@@ -5,27 +5,28 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole\Documents\Psychobiologie\Minor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole\Documents\Psychobiologie\Minor\GitHub RushHour\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Results Rush Hour Sol" sheetId="1" r:id="rId1"/>
     <sheet name="iteraties per bord" sheetId="2" r:id="rId2"/>
-    <sheet name="moves + iteraties bord 1" sheetId="4" r:id="rId3"/>
-    <sheet name="moves + iteraties bord 3" sheetId="6" r:id="rId4"/>
-    <sheet name="Blad6" sheetId="7" r:id="rId5"/>
-    <sheet name="moves + iteraties bord 2" sheetId="5" r:id="rId6"/>
-    <sheet name="moves per bord" sheetId="3" r:id="rId7"/>
+    <sheet name="Blad1" sheetId="8" r:id="rId3"/>
+    <sheet name="moves + iteraties bord 1" sheetId="4" r:id="rId4"/>
+    <sheet name="moves + iteraties bord 3" sheetId="6" r:id="rId5"/>
+    <sheet name="moves + iteraties bord 4" sheetId="7" r:id="rId6"/>
+    <sheet name="moves + iteraties bord 2" sheetId="5" r:id="rId7"/>
+    <sheet name="moves per bord" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="29">
   <si>
     <t>Results Rush Hour Solving Algorithms</t>
   </si>
@@ -275,7 +276,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -315,10 +316,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -394,6 +398,10 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFF28A00"/>
+      <color rgb="FFFFB965"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -915,7 +923,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1248,12 +1255,12 @@
         <c:gapWidth val="0"/>
         <c:gapDepth val="308"/>
         <c:shape val="box"/>
-        <c:axId val="369430632"/>
-        <c:axId val="369432592"/>
+        <c:axId val="308867720"/>
+        <c:axId val="121620152"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="369430632"/>
+        <c:axId val="308867720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1290,7 +1297,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="369432592"/>
+        <c:crossAx val="121620152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1298,7 +1305,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="369432592"/>
+        <c:axId val="121620152"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1350,7 +1357,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="369430632"/>
+        <c:crossAx val="308867720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1440,6 +1447,1776 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL" sz="2400"/>
+              <a:t>Zetten</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="nl-NL" sz="2400" baseline="0"/>
+              <a:t> en iteraties voor alle borden en alle algoritmes</a:t>
+            </a:r>
+            <a:endParaRPr lang="nl-NL" sz="2400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14759954865572578"/>
+          <c:y val="0.17418933451573754"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Zetten</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFB965"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFB965"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFB965"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.394286422870325E-18"/>
+                  <c:y val="4.6421663442939944E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="4.6421663442939944E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="4.6421663442939944E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="4.6421663442940041E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.35771456914813E-17"/>
+                  <c:y val="4.6421663442940041E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="4.6421663442940041E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="4.6421663442940041E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="4.6421663442939944E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="4.6421663442940041E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.71542913829626E-17"/>
+                  <c:y val="4.3842682140554388E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.71542913829626E-17"/>
+                  <c:y val="4.6421663442939944E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.71542913829626E-17"/>
+                  <c:y val="4.6421663442940041E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5267702936097731E-3"/>
+                  <c:y val="4.6421732074743094E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.7358634768355102E-3"/>
+                  <c:y val="4.6421697287838952E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Blad1!$B$7:$S$8</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="18"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>BFS</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>A*</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Beam Search</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>BFS</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>A*</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Beam Search</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>BFS</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>A*</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Beam Search</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>BFS</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>A*</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Beam Search</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>BFS</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>A*</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Beam Search</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>BFS</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>A*</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Beam Search</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Bord 1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Bord 2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Bord 3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Bord 4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Bord 5</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Bord 6</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$B$9:$S$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>832</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7195</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1759</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Iteraties</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="F28A00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="F28A00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="F28A00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.7472527472527475E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.6630036630036799E-3"/>
+                  <c:y val="-4.7280777685490106E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.7472527472527475E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.663003663003663E-3"/>
+                  <c:y val="-4.7280777685490106E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.7472527472527136E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.7472527472527475E-3"/>
+                  <c:y val="-4.7280777685490106E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.8315018315018315E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.7472527472527475E-3"/>
+                  <c:y val="-2.5789813023855577E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.663003663003663E-3"/>
+                  <c:y val="-9.4561555370980212E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.7472527472527475E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.663003663003663E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.7472527472527475E-3"/>
+                  <c:y val="-2.5789813023855577E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.4945054945054949E-3"/>
+                  <c:y val="-4.7280777685490106E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.747252747252613E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Blad1!$B$7:$S$8</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="18"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>BFS</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>A*</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Beam Search</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>BFS</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>A*</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Beam Search</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>BFS</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>A*</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Beam Search</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>BFS</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>A*</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Beam Search</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>BFS</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>A*</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Beam Search</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>BFS</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>A*</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Beam Search</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Bord 1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Bord 2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Bord 3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Bord 4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Bord 5</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Bord 6</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$B$10:$S$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>8600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6927</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3830</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3551</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1816</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>567</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>435</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>386</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>290406</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>130287</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>46661</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>324411</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>120935</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="398382608"/>
+        <c:axId val="398383000"/>
+        <c:axId val="401719664"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="398382608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="398383000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="398383000"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="398382608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="401719664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="1" u="none" strike="noStrike" kern="1200" cap="none" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="398383000"/>
+        <c:crosses val="autoZero"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:serAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="nl-NL"/>
@@ -1689,7 +3466,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1868,7 +3644,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1933,12 +3708,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="418162560"/>
-        <c:axId val="418164128"/>
-        <c:axId val="420071112"/>
+        <c:axId val="309789680"/>
+        <c:axId val="309776152"/>
+        <c:axId val="308697824"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="418162560"/>
+        <c:axId val="309789680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1975,7 +3750,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418164128"/>
+        <c:crossAx val="309776152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1983,7 +3758,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="418164128"/>
+        <c:axId val="309776152"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2035,12 +3810,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418162560"/>
+        <c:crossAx val="309789680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="420071112"/>
+        <c:axId val="308697824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2049,7 +3824,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="418164128"/>
+        <c:crossAx val="309776152"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -2129,7 +3904,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="nl-NL"/>
@@ -2372,7 +4147,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2551,7 +4325,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2616,12 +4389,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="370897280"/>
-        <c:axId val="370894144"/>
-        <c:axId val="298729232"/>
+        <c:axId val="309778616"/>
+        <c:axId val="310547240"/>
+        <c:axId val="310512720"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="370897280"/>
+        <c:axId val="309778616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2658,7 +4431,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="370894144"/>
+        <c:crossAx val="310547240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2666,7 +4439,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="370894144"/>
+        <c:axId val="310547240"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2718,12 +4491,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="370897280"/>
+        <c:crossAx val="309778616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="298729232"/>
+        <c:axId val="310512720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2732,7 +4505,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="370894144"/>
+        <c:crossAx val="310547240"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -2812,7 +4585,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="nl-NL"/>
@@ -2933,7 +4706,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad6!$B$1</c:f>
+              <c:f>'moves + iteraties bord 4'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3055,7 +4828,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3076,7 +4848,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Blad6!$A$2:$A$4</c:f>
+              <c:f>'moves + iteraties bord 4'!$A$2:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3093,7 +4865,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad6!$B$2:$B$4</c:f>
+              <c:f>'moves + iteraties bord 4'!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3115,7 +4887,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad6!$C$1</c:f>
+              <c:f>'moves + iteraties bord 4'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3234,7 +5006,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3255,7 +5026,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Blad6!$A$2:$A$4</c:f>
+              <c:f>'moves + iteraties bord 4'!$A$2:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3272,7 +5043,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad6!$C$2:$C$4</c:f>
+              <c:f>'moves + iteraties bord 4'!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3299,12 +5070,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="410639064"/>
-        <c:axId val="410637496"/>
-        <c:axId val="419973016"/>
+        <c:axId val="122150960"/>
+        <c:axId val="122150568"/>
+        <c:axId val="310516960"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="410639064"/>
+        <c:axId val="122150960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3341,7 +5112,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="410637496"/>
+        <c:crossAx val="122150568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3349,7 +5120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="410637496"/>
+        <c:axId val="122150568"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3401,12 +5172,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="410639064"/>
+        <c:crossAx val="122150960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="419973016"/>
+        <c:axId val="310516960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3415,7 +5186,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="410637496"/>
+        <c:crossAx val="122150568"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -3495,7 +5266,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="nl-NL"/>
@@ -3745,7 +5516,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3924,7 +5694,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3989,12 +5758,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="418615456"/>
-        <c:axId val="418623296"/>
-        <c:axId val="298727112"/>
+        <c:axId val="122151352"/>
+        <c:axId val="310261864"/>
+        <c:axId val="310514416"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="418615456"/>
+        <c:axId val="122151352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4031,7 +5800,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418623296"/>
+        <c:crossAx val="310261864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4039,7 +5808,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="418623296"/>
+        <c:axId val="310261864"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4091,12 +5860,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418615456"/>
+        <c:crossAx val="122151352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="298727112"/>
+        <c:axId val="310514416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4105,7 +5874,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="418623296"/>
+        <c:crossAx val="310261864"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -4185,7 +5954,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="nl-NL"/>
@@ -4846,12 +6615,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="418159424"/>
-        <c:axId val="418160600"/>
+        <c:axId val="310262256"/>
+        <c:axId val="310262648"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="418159424"/>
+        <c:axId val="310262256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4888,7 +6657,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418160600"/>
+        <c:crossAx val="310262648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4896,7 +6665,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="418160600"/>
+        <c:axId val="310262648"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4948,7 +6717,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418159424"/>
+        <c:crossAx val="310262256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5277,6 +7046,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
@@ -8241,19 +10050,513 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>381001</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323851</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>423863</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>366713</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8280,20 +10583,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Grafiek 1"/>
+        <xdr:cNvPr id="4" name="Grafiek 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8316,15 +10619,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8417,6 +10720,41 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -9560,11 +11898,11 @@
   </sheetPr>
   <dimension ref="A1:IV23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F13" activeCellId="1" sqref="C13:D13 F13"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9573,15 +11911,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -9892,7 +12230,7 @@
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
-      <c r="F17" s="14">
+      <c r="F17" s="13">
         <v>2500270</v>
       </c>
       <c r="G17" s="12"/>
@@ -9933,7 +12271,7 @@
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
-      <c r="F20" s="14">
+      <c r="F20" s="13">
         <v>1035075</v>
       </c>
       <c r="G20" s="12"/>
@@ -9989,8 +12327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10134,58 +12472,345 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>27</v>
       </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B2">
+      <c r="B3">
+        <v>8600</v>
+      </c>
+      <c r="C3">
         <v>83</v>
       </c>
-      <c r="C2">
+      <c r="D3">
+        <v>3551</v>
+      </c>
+      <c r="E3">
+        <v>29</v>
+      </c>
+      <c r="F3">
+        <v>486</v>
+      </c>
+      <c r="G3">
+        <v>35</v>
+      </c>
+      <c r="H3">
+        <v>290406</v>
+      </c>
+      <c r="I3" s="9">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>6927</v>
+      </c>
+      <c r="C4">
+        <v>83</v>
+      </c>
+      <c r="D4">
+        <v>1816</v>
+      </c>
+      <c r="E4">
+        <v>29</v>
+      </c>
+      <c r="F4">
+        <v>435</v>
+      </c>
+      <c r="G4">
+        <v>37</v>
+      </c>
+      <c r="H4">
+        <v>130287</v>
+      </c>
+      <c r="I4" s="9">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>3830</v>
+      </c>
+      <c r="C5">
+        <v>85</v>
+      </c>
+      <c r="D5">
+        <v>567</v>
+      </c>
+      <c r="E5">
+        <v>31</v>
+      </c>
+      <c r="F5">
+        <v>386</v>
+      </c>
+      <c r="G5">
+        <v>38</v>
+      </c>
+      <c r="H5">
+        <v>46661</v>
+      </c>
+      <c r="I5" s="9">
+        <v>832</v>
+      </c>
+      <c r="J5" s="12">
+        <v>324411</v>
+      </c>
+      <c r="K5" s="12">
+        <v>7195</v>
+      </c>
+      <c r="L5" s="12">
+        <v>120935</v>
+      </c>
+      <c r="M5" s="12">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>17</v>
+      </c>
+      <c r="R8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>83</v>
+      </c>
+      <c r="C9">
+        <v>83</v>
+      </c>
+      <c r="D9">
+        <v>85</v>
+      </c>
+      <c r="E9">
+        <v>29</v>
+      </c>
+      <c r="F9">
+        <v>29</v>
+      </c>
+      <c r="G9">
+        <v>31</v>
+      </c>
+      <c r="H9">
+        <v>35</v>
+      </c>
+      <c r="I9">
+        <v>37</v>
+      </c>
+      <c r="J9">
+        <v>38</v>
+      </c>
+      <c r="K9" s="9">
+        <v>51</v>
+      </c>
+      <c r="L9">
+        <v>53</v>
+      </c>
+      <c r="M9">
+        <v>832</v>
+      </c>
+      <c r="P9" s="12">
+        <v>7195</v>
+      </c>
+      <c r="S9" s="12">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10">
         <v>8600</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3">
-        <v>83</v>
-      </c>
-      <c r="C3">
+      <c r="C10">
         <v>6927</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4">
-        <v>115</v>
-      </c>
-      <c r="C4">
+      <c r="D10">
         <v>3830</v>
+      </c>
+      <c r="E10">
+        <v>3551</v>
+      </c>
+      <c r="F10">
+        <v>1816</v>
+      </c>
+      <c r="G10">
+        <v>567</v>
+      </c>
+      <c r="H10">
+        <v>486</v>
+      </c>
+      <c r="I10">
+        <v>435</v>
+      </c>
+      <c r="J10">
+        <v>386</v>
+      </c>
+      <c r="K10">
+        <v>290406</v>
+      </c>
+      <c r="L10">
+        <v>130287</v>
+      </c>
+      <c r="M10">
+        <v>46661</v>
+      </c>
+      <c r="P10" s="12">
+        <v>324411</v>
+      </c>
+      <c r="S10" s="12">
+        <v>120935</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10194,7 +12819,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10212,21 +12837,21 @@
         <v>17</v>
       </c>
       <c r="B2">
-        <v>35</v>
-      </c>
-      <c r="C2" s="9">
-        <v>486</v>
+        <v>83</v>
+      </c>
+      <c r="C2">
+        <v>8600</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B3">
-        <v>37</v>
-      </c>
-      <c r="C3" s="9">
-        <v>435</v>
+        <v>83</v>
+      </c>
+      <c r="C3">
+        <v>6927</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
@@ -10234,10 +12859,10 @@
         <v>25</v>
       </c>
       <c r="B4">
-        <v>38</v>
-      </c>
-      <c r="C4" s="9">
-        <v>386</v>
+        <v>115</v>
+      </c>
+      <c r="C4">
+        <v>3830</v>
       </c>
     </row>
   </sheetData>
@@ -10251,7 +12876,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10268,33 +12893,33 @@
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="9">
-        <v>51</v>
+      <c r="B2">
+        <v>35</v>
       </c>
       <c r="C2" s="9">
-        <v>290406</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="9">
-        <v>53</v>
+      <c r="B3">
+        <v>37</v>
       </c>
       <c r="C3" s="9">
-        <v>130287</v>
+        <v>435</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="9">
-        <v>832</v>
+      <c r="B4">
+        <v>38</v>
       </c>
       <c r="C4" s="9">
-        <v>46661</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -10307,8 +12932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10325,33 +12950,33 @@
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2">
-        <v>29</v>
-      </c>
-      <c r="C2">
-        <v>3551</v>
+      <c r="B2" s="9">
+        <v>51</v>
+      </c>
+      <c r="C2" s="9">
+        <v>290406</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3">
-        <v>29</v>
-      </c>
-      <c r="C3">
-        <v>1816</v>
+        <v>28</v>
+      </c>
+      <c r="B3" s="9">
+        <v>53</v>
+      </c>
+      <c r="C3" s="9">
+        <v>130287</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4">
-        <v>31</v>
-      </c>
-      <c r="C4">
-        <v>567</v>
+      <c r="B4" s="9">
+        <v>832</v>
+      </c>
+      <c r="C4" s="9">
+        <v>46661</v>
       </c>
     </row>
   </sheetData>
@@ -10361,6 +12986,63 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>3551</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>567</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>

</xml_diff>